<commit_message>
Toolbar - Items : Changed to xpath from id
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Toolbars.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Toolbars.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>textbox</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Toolbar - Items</t>
   </si>
   <si>
-    <t>Ribbon.ListItem-title</t>
-  </si>
-  <si>
     <t>Toolbar - Items - Start New Tranmittal</t>
   </si>
   <si>
@@ -167,6 +164,12 @@
   </si>
   <si>
     <t>element_notdisplayed</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>.//*[@id='Ribbon.ListItem-title']/a</t>
   </si>
 </sst>
 </file>
@@ -741,37 +744,37 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -841,18 +846,18 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -861,7 +866,7 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toolbar - Items - changed from xpath to id and locator accordingly.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Toolbars.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Toolbars.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>textbox</t>
   </si>
@@ -166,10 +166,7 @@
     <t>element_notdisplayed</t>
   </si>
   <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>.//*[@id='Ribbon.ListItem-title']/a</t>
+    <t>Ribbon.ListItem-title</t>
   </si>
 </sst>
 </file>
@@ -793,9 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -846,13 +841,13 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">

</xml_diff>